<commit_message>
cleanup for final version
</commit_message>
<xml_diff>
--- a/src/lithium/data/lithiumMars-juin 2017 NHE1.xlsx
+++ b/src/lithium/data/lithiumMars-juin 2017 NHE1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32780" windowHeight="18660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +405,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,7 +570,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -712,6 +718,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="137" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="144">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -978,22 +1005,22 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
-                <c:pt idx="3" formatCode="0.0">
+                <c:pt idx="3" formatCode="#,#00">
                   <c:v>-8.771987800000001</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.0">
+                <c:pt idx="4" formatCode="#,#00">
                   <c:v>-8.7024606</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.0">
+                <c:pt idx="6" formatCode="#,#00">
                   <c:v>-13.1915437</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.0">
+                <c:pt idx="8" formatCode="#,#00">
                   <c:v>-12.9250522</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.0">
+                <c:pt idx="10" formatCode="#,#00">
                   <c:v>-12.8275887</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="0.0">
+                <c:pt idx="17" formatCode="#,#00">
                   <c:v>-12.9629817</c:v>
                 </c:pt>
               </c:numCache>
@@ -1143,11 +1170,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2039838424"/>
-        <c:axId val="-2142643912"/>
+        <c:axId val="2048898696"/>
+        <c:axId val="2038243944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2039838424"/>
+        <c:axId val="2048898696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130.0"/>
@@ -1185,12 +1212,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="-2142643912"/>
+        <c:crossAx val="2038243944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142643912"/>
+        <c:axId val="2038243944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-6.0"/>
@@ -1227,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2039838424"/>
+        <c:crossAx val="2048898696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1342,7 +1369,7 @@
             <c:numRef>
               <c:f>Feuil1!$K$37:$K$51</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
                   <c:v>-11.6644118</c:v>
@@ -1478,11 +1505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142552152"/>
-        <c:axId val="2039584968"/>
+        <c:axId val="2038336280"/>
+        <c:axId val="2038341976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142552152"/>
+        <c:axId val="2038336280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3700.0"/>
@@ -1525,12 +1552,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="2039584968"/>
+        <c:crossAx val="2038341976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2039584968"/>
+        <c:axId val="2038341976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,11 +1589,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142552152"/>
+        <c:crossAx val="2038336280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1634,7 +1661,7 @@
             <c:numRef>
               <c:f>Feuil1!$G$37:$G$47</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.259365994236311</c:v>
@@ -1658,7 +1685,7 @@
             <c:numRef>
               <c:f>Feuil1!$K$37:$K$47</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
                   <c:v>-11.6644118</c:v>
@@ -1779,11 +1806,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142874120"/>
-        <c:axId val="2123640680"/>
+        <c:axId val="2047949480"/>
+        <c:axId val="2047943704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142874120"/>
+        <c:axId val="2047949480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,16 +1847,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="2123640680"/>
+        <c:crossAx val="2047943704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2123640680"/>
+        <c:axId val="2047943704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1861,11 +1888,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142874120"/>
+        <c:crossAx val="2047949480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1948,19 +1975,19 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
-                <c:pt idx="0" formatCode="0.0">
+                <c:pt idx="0" formatCode="#,#00">
                   <c:v>5.072046109510086</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.0">
+                <c:pt idx="3" formatCode="#,#00">
                   <c:v>25.36023054755043</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.0">
+                <c:pt idx="5" formatCode="#,#00">
                   <c:v>23.05475504322767</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.0">
+                <c:pt idx="7" formatCode="#,#00">
                   <c:v>23.63112391930836</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.0">
+                <c:pt idx="14" formatCode="#,#00">
                   <c:v>22.47838616714698</c:v>
                 </c:pt>
               </c:numCache>
@@ -1970,7 +1997,7 @@
             <c:numRef>
               <c:f>Feuil1!$K$20:$K$34</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-8.771987800000001</c:v>
@@ -2214,11 +2241,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2142434328"/>
-        <c:axId val="-2142553736"/>
+        <c:axId val="2047961208"/>
+        <c:axId val="2047974824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2142434328"/>
+        <c:axId val="2047961208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2250,16 +2277,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="-2142553736"/>
+        <c:crossAx val="2047974824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142553736"/>
+        <c:axId val="2047974824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-8.0"/>
@@ -2297,11 +2324,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142434328"/>
+        <c:crossAx val="2047961208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2807,11 +2834,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2117649208"/>
-        <c:axId val="2125965960"/>
+        <c:axId val="2047884344"/>
+        <c:axId val="2047876776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2117649208"/>
+        <c:axId val="2047884344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,12 +2872,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125965960"/>
+        <c:crossAx val="2047876776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2125965960"/>
+        <c:axId val="2047876776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117649208"/>
+        <c:crossAx val="2047884344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3167,11 +3194,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2117277784"/>
-        <c:axId val="2130334648"/>
+        <c:axId val="-2116933992"/>
+        <c:axId val="-2116931000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2117277784"/>
+        <c:axId val="-2116933992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3181,12 +3208,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130334648"/>
+        <c:crossAx val="-2116931000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130334648"/>
+        <c:axId val="-2116931000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3196,11 +3223,133 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117277784"/>
+        <c:crossAx val="-2116933992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$O$38:$O$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>229.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>485.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>394.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>794.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2181.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2341.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2050139400"/>
+        <c:axId val="2136935928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2050139400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2136935928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2136935928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2050139400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3449,15 +3598,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3471,6 +3620,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Graphique 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3975,8 +4154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38:S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6646,53 +6825,65 @@
       <c r="A134">
         <v>15</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="59">
         <v>0</v>
       </c>
-      <c r="C134" s="24" t="s">
+      <c r="C134" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D134" s="20"/>
-      <c r="G134" s="40"/>
-      <c r="H134" s="40"/>
-      <c r="I134" s="48"/>
-      <c r="J134" s="48"/>
-      <c r="K134" s="43"/>
+      <c r="D134" s="59"/>
+      <c r="E134" s="59"/>
+      <c r="F134" s="59"/>
+      <c r="G134" s="61"/>
+      <c r="H134" s="61"/>
+      <c r="I134" s="62"/>
+      <c r="J134" s="62"/>
+      <c r="K134" s="59"/>
     </row>
     <row r="135" spans="1:22">
       <c r="A135">
         <v>15</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="59">
         <v>15</v>
       </c>
-      <c r="C135" s="24" t="s">
+      <c r="C135" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="D135" s="35" t="s">
+      <c r="D135" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="E135">
+      <c r="E135" s="59">
         <v>229</v>
       </c>
-      <c r="F135" s="4">
+      <c r="F135" s="63">
         <v>458</v>
       </c>
-      <c r="G135" s="38">
+      <c r="G135" s="63">
         <v>65.994236311239206</v>
       </c>
-      <c r="H135" s="47">
+      <c r="H135" s="64">
         <v>4.399615754082614E-3</v>
       </c>
-      <c r="I135" s="48">
+      <c r="I135" s="62">
         <v>1.42</v>
       </c>
-      <c r="J135" s="48"/>
-      <c r="K135" s="43">
+      <c r="J135" s="62"/>
+      <c r="K135" s="59">
         <v>-13.93</v>
       </c>
     </row>
     <row r="136" spans="1:22">
+      <c r="B136" s="59"/>
+      <c r="C136" s="59"/>
+      <c r="D136" s="59"/>
+      <c r="E136" s="59"/>
+      <c r="F136" s="59"/>
+      <c r="G136" s="59"/>
+      <c r="H136" s="59"/>
+      <c r="I136" s="59"/>
+      <c r="J136" s="59"/>
+      <c r="K136" s="59"/>
       <c r="L136">
         <v>15</v>
       </c>
@@ -6726,6 +6917,16 @@
       </c>
     </row>
     <row r="137" spans="1:22">
+      <c r="B137" s="59"/>
+      <c r="C137" s="59"/>
+      <c r="D137" s="59"/>
+      <c r="E137" s="59"/>
+      <c r="F137" s="59"/>
+      <c r="G137" s="59"/>
+      <c r="H137" s="59"/>
+      <c r="I137" s="59"/>
+      <c r="J137" s="59"/>
+      <c r="K137" s="59"/>
       <c r="M137">
         <v>15</v>
       </c>
@@ -6759,32 +6960,32 @@
       <c r="A138">
         <v>15</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="59">
         <v>30</v>
       </c>
-      <c r="C138" s="24" t="s">
+      <c r="C138" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="D138" s="35" t="s">
+      <c r="D138" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="E138">
+      <c r="E138" s="59">
         <v>485</v>
       </c>
-      <c r="F138" s="4">
+      <c r="F138" s="63">
         <v>970</v>
       </c>
-      <c r="G138" s="38">
+      <c r="G138" s="63">
         <v>139.76945244956772</v>
       </c>
-      <c r="H138" s="47">
+      <c r="H138" s="64">
         <v>9.3179634966378492E-3</v>
       </c>
-      <c r="I138" s="48">
+      <c r="I138" s="62">
         <v>1.4</v>
       </c>
-      <c r="J138" s="48"/>
-      <c r="K138" s="43">
+      <c r="J138" s="62"/>
+      <c r="K138" s="59">
         <v>-13.95</v>
       </c>
     </row>
@@ -6792,19 +6993,30 @@
       <c r="A139">
         <v>15</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="59">
         <v>30</v>
       </c>
-      <c r="C139" s="24"/>
-      <c r="D139" s="35"/>
-      <c r="F139" s="4"/>
-      <c r="G139" s="39"/>
-      <c r="H139" s="39"/>
-      <c r="I139" s="48"/>
-      <c r="J139" s="48"/>
-      <c r="K139" s="43"/>
+      <c r="C139" s="60"/>
+      <c r="D139" s="62"/>
+      <c r="E139" s="59"/>
+      <c r="F139" s="63"/>
+      <c r="G139" s="59"/>
+      <c r="H139" s="59"/>
+      <c r="I139" s="62"/>
+      <c r="J139" s="62"/>
+      <c r="K139" s="59"/>
     </row>
     <row r="140" spans="1:22">
+      <c r="B140" s="59"/>
+      <c r="C140" s="59"/>
+      <c r="D140" s="59"/>
+      <c r="E140" s="59"/>
+      <c r="F140" s="59"/>
+      <c r="G140" s="59"/>
+      <c r="H140" s="59"/>
+      <c r="I140" s="59"/>
+      <c r="J140" s="59"/>
+      <c r="K140" s="59"/>
       <c r="L140">
         <v>15</v>
       </c>
@@ -6841,62 +7053,66 @@
       <c r="A141">
         <v>15</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="59">
         <v>45</v>
       </c>
-      <c r="C141" s="24"/>
-      <c r="D141" s="35"/>
-      <c r="G141" s="39"/>
-      <c r="H141" s="39"/>
-      <c r="I141" s="48"/>
-      <c r="J141" s="48"/>
-      <c r="K141" s="43"/>
+      <c r="C141" s="60"/>
+      <c r="D141" s="62"/>
+      <c r="E141" s="59"/>
+      <c r="F141" s="59"/>
+      <c r="G141" s="59"/>
+      <c r="H141" s="59"/>
+      <c r="I141" s="62"/>
+      <c r="J141" s="62"/>
+      <c r="K141" s="59"/>
     </row>
     <row r="142" spans="1:22">
       <c r="A142">
         <v>15</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="59">
         <v>45</v>
       </c>
-      <c r="C142" s="24"/>
-      <c r="D142" s="35"/>
-      <c r="G142" s="39"/>
-      <c r="H142" s="39"/>
-      <c r="I142" s="48"/>
-      <c r="J142" s="48"/>
-      <c r="K142" s="43"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="62"/>
+      <c r="E142" s="59"/>
+      <c r="F142" s="59"/>
+      <c r="G142" s="59"/>
+      <c r="H142" s="59"/>
+      <c r="I142" s="62"/>
+      <c r="J142" s="62"/>
+      <c r="K142" s="59"/>
     </row>
     <row r="143" spans="1:22">
       <c r="A143">
         <v>15</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="59">
         <v>60</v>
       </c>
-      <c r="C143" s="24" t="s">
+      <c r="C143" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="D143" s="35" t="s">
+      <c r="D143" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="59">
         <v>794</v>
       </c>
-      <c r="F143" s="4">
+      <c r="F143" s="63">
         <v>1588</v>
       </c>
-      <c r="G143" s="38">
+      <c r="G143" s="63">
         <v>228.81844380403459</v>
       </c>
-      <c r="H143" s="47">
+      <c r="H143" s="64">
         <v>1.5254562920268973E-2</v>
       </c>
-      <c r="I143" s="48">
+      <c r="I143" s="62">
         <v>2.54</v>
       </c>
-      <c r="J143" s="48"/>
-      <c r="K143" s="43">
+      <c r="J143" s="62"/>
+      <c r="K143" s="59">
         <v>-12.809999999999999</v>
       </c>
     </row>
@@ -6904,142 +7120,149 @@
       <c r="A144">
         <v>15</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="59">
         <v>60</v>
       </c>
-      <c r="C144" s="24"/>
-      <c r="D144" s="35"/>
-      <c r="G144" s="39"/>
-      <c r="H144" s="39"/>
-      <c r="I144" s="48"/>
-      <c r="J144" s="48"/>
-      <c r="K144" s="43"/>
+      <c r="C144" s="60"/>
+      <c r="D144" s="62"/>
+      <c r="E144" s="59"/>
+      <c r="F144" s="59"/>
+      <c r="G144" s="59"/>
+      <c r="H144" s="59"/>
+      <c r="I144" s="62"/>
+      <c r="J144" s="62"/>
+      <c r="K144" s="59"/>
     </row>
     <row r="145" spans="1:11">
       <c r="A145">
         <v>15</v>
       </c>
-      <c r="C145" s="24"/>
-      <c r="D145" s="35"/>
-      <c r="G145" s="39"/>
-      <c r="H145" s="39"/>
-      <c r="I145" s="48"/>
-      <c r="J145" s="48"/>
-      <c r="K145" s="43"/>
+      <c r="B145" s="59"/>
+      <c r="C145" s="60"/>
+      <c r="D145" s="62"/>
+      <c r="E145" s="59"/>
+      <c r="F145" s="59"/>
+      <c r="G145" s="59"/>
+      <c r="H145" s="59"/>
+      <c r="I145" s="62"/>
+      <c r="J145" s="62"/>
+      <c r="K145" s="59"/>
     </row>
     <row r="146" spans="1:11">
-      <c r="B146">
+      <c r="B146" s="59">
         <v>300</v>
       </c>
-      <c r="C146" s="24" t="s">
+      <c r="C146" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="D146" s="35" t="s">
+      <c r="D146" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="E146">
+      <c r="E146" s="59">
         <v>2181</v>
       </c>
-      <c r="F146" s="4">
+      <c r="F146" s="63">
         <v>4362</v>
       </c>
-      <c r="G146" s="38">
+      <c r="G146" s="63">
         <v>628.53025936599431</v>
       </c>
-      <c r="H146" s="47">
+      <c r="H146" s="64">
         <v>4.1902017291066282E-2</v>
       </c>
-      <c r="I146" s="48">
+      <c r="I146" s="62">
         <v>7.54</v>
       </c>
-      <c r="J146" s="48"/>
-      <c r="K146" s="43">
+      <c r="J146" s="62"/>
+      <c r="K146" s="59">
         <v>-7.81</v>
       </c>
     </row>
     <row r="147" spans="1:11">
-      <c r="B147">
+      <c r="B147" s="59">
         <v>900</v>
       </c>
-      <c r="C147" s="24" t="s">
+      <c r="C147" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="D147" s="35" t="s">
+      <c r="D147" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="E147">
+      <c r="E147" s="59">
         <v>2341</v>
       </c>
-      <c r="F147" s="4">
+      <c r="F147" s="63">
         <v>4682</v>
       </c>
-      <c r="G147" s="38">
+      <c r="G147" s="63">
         <v>674.63976945244951</v>
       </c>
-      <c r="H147" s="47">
+      <c r="H147" s="64">
         <v>4.49759846301633E-2</v>
       </c>
-      <c r="I147" s="48">
+      <c r="I147" s="62">
         <v>12.64</v>
       </c>
-      <c r="J147" s="48"/>
-      <c r="K147" s="43">
+      <c r="J147" s="62"/>
+      <c r="K147" s="59">
         <v>-2.7099999999999991</v>
       </c>
     </row>
     <row r="148" spans="1:11">
-      <c r="B148">
+      <c r="B148" s="59">
         <v>3600</v>
       </c>
-      <c r="C148" s="24" t="s">
+      <c r="C148" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="D148" s="35" t="s">
+      <c r="D148" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="E148" s="45">
+      <c r="E148" s="59">
         <v>1381</v>
       </c>
-      <c r="F148" s="46">
+      <c r="F148" s="63">
         <v>2762</v>
       </c>
-      <c r="G148" s="38">
+      <c r="G148" s="63">
         <v>397.98270893371756</v>
       </c>
-      <c r="H148" s="47">
+      <c r="H148" s="64">
         <v>2.653218059558117E-2</v>
       </c>
-      <c r="I148" s="48">
+      <c r="I148" s="62">
         <v>15.13</v>
       </c>
-      <c r="J148" s="48"/>
-      <c r="K148" s="43">
+      <c r="J148" s="62"/>
+      <c r="K148" s="59">
         <v>-0.21999999999999886</v>
       </c>
     </row>
     <row r="149" spans="1:11">
-      <c r="D149" s="48" t="s">
+      <c r="B149" s="59"/>
+      <c r="C149" s="59"/>
+      <c r="D149" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="E149" s="45">
+      <c r="E149" s="59">
         <v>1381</v>
       </c>
-      <c r="F149" s="46">
+      <c r="F149" s="63">
         <v>2762</v>
       </c>
-      <c r="G149" s="38">
+      <c r="G149" s="63">
         <v>397.98270893371756</v>
       </c>
-      <c r="H149" s="47">
+      <c r="H149" s="64">
         <v>2.653218059558117E-2</v>
       </c>
-      <c r="I149" s="49">
+      <c r="I149" s="65">
         <v>14.981471000000001</v>
       </c>
-      <c r="J149" s="50">
+      <c r="J149" s="66">
         <v>2.1293106999999999E-2</v>
       </c>
-      <c r="K149" s="56">
+      <c r="K149" s="67">
         <v>-0.36852899999999877</v>
       </c>
     </row>

</xml_diff>